<commit_message>
item update with tax
</commit_message>
<xml_diff>
--- a/LSL/Transactional Data/Management Reports/task-list.xlsx
+++ b/LSL/Transactional Data/Management Reports/task-list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="311">
   <si>
     <t>.Timestamp from PBSA is defaukt and it is 00:00:00</t>
   </si>
@@ -939,6 +939,24 @@
   </si>
   <si>
     <t>XXPBSA_ENDPOINTS - outlet - connectivity\11th week</t>
+  </si>
+  <si>
+    <t>Sup. ret. weighted avg confirmation/</t>
+  </si>
+  <si>
+    <t>partial grn from same po/</t>
+  </si>
+  <si>
+    <t>ap invoice batch testing/</t>
+  </si>
+  <si>
+    <t>sequence+with outletid in sales\pay/-db sequence used</t>
+  </si>
+  <si>
+    <t>po screen - re-named column for ship to location instead of dff/</t>
+  </si>
+  <si>
+    <t>identify warehouse -&gt; outlet transfer from a notification sent based on the inter-stock and Hold payment till inter-stock doneX</t>
   </si>
 </sst>
 </file>
@@ -1260,11 +1278,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D313"/>
+  <dimension ref="A1:D319"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A225" workbookViewId="0">
-      <selection activeCell="C275" sqref="C275"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5151,7 +5167,7 @@
         <v>810626</v>
       </c>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>277</v>
       </c>
@@ -5165,7 +5181,7 @@
         <v>810626</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>278</v>
       </c>
@@ -5179,7 +5195,7 @@
         <v>810626</v>
       </c>
     </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>279</v>
       </c>
@@ -5207,7 +5223,7 @@
         <v>810626</v>
       </c>
     </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>281</v>
       </c>
@@ -5221,7 +5237,7 @@
         <v>810626</v>
       </c>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>282</v>
       </c>
@@ -5249,7 +5265,7 @@
         <v>810626</v>
       </c>
     </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>284</v>
       </c>
@@ -5263,7 +5279,7 @@
         <v>810626</v>
       </c>
     </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>285</v>
       </c>
@@ -5277,7 +5293,7 @@
         <v>810626</v>
       </c>
     </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>286</v>
       </c>
@@ -5291,7 +5307,7 @@
         <v>810626</v>
       </c>
     </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>287</v>
       </c>
@@ -5333,7 +5349,7 @@
         <v>810626</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>290</v>
       </c>
@@ -5459,7 +5475,7 @@
         <v>810626</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>299</v>
       </c>
@@ -5473,7 +5489,7 @@
         <v>810626</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>300</v>
       </c>
@@ -5487,7 +5503,7 @@
         <v>810626</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>301</v>
       </c>
@@ -5515,7 +5531,7 @@
         <v>810626</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>303</v>
       </c>
@@ -5529,7 +5545,7 @@
         <v>810626</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>304</v>
       </c>
@@ -5543,7 +5559,7 @@
         <v>810626</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>305</v>
       </c>
@@ -5571,7 +5587,7 @@
         <v>810626</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>307</v>
       </c>
@@ -5641,7 +5657,7 @@
         <v>810626</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>312</v>
       </c>
@@ -5652,6 +5668,90 @@
         <v>810565</v>
       </c>
       <c r="D313" s="2">
+        <v>810626</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A314">
+        <v>313</v>
+      </c>
+      <c r="B314" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C314" s="2">
+        <v>810626</v>
+      </c>
+      <c r="D314" s="2">
+        <v>810626</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A315">
+        <v>314</v>
+      </c>
+      <c r="B315" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C315" s="2">
+        <v>810626</v>
+      </c>
+      <c r="D315" s="2">
+        <v>810626</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A316">
+        <v>315</v>
+      </c>
+      <c r="B316" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C316" s="2">
+        <v>810626</v>
+      </c>
+      <c r="D316" s="2">
+        <v>810626</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A317">
+        <v>316</v>
+      </c>
+      <c r="B317" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C317" s="2">
+        <v>810626</v>
+      </c>
+      <c r="D317" s="2">
+        <v>810626</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A318">
+        <v>317</v>
+      </c>
+      <c r="B318" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C318" s="2">
+        <v>810626</v>
+      </c>
+      <c r="D318" s="2">
+        <v>810626</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A319">
+        <v>318</v>
+      </c>
+      <c r="B319" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C319" s="2">
+        <v>810626</v>
+      </c>
+      <c r="D319" s="2">
         <v>810626</v>
       </c>
     </row>

</xml_diff>